<commit_message>
Adding PowerPoint and unsaved changes to Eval spreadsheet
</commit_message>
<xml_diff>
--- a/Git GUIs Eval.xlsx
+++ b/Git GUIs Eval.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861CF904-8320-4CE0-A222-5D40FA3E3DB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5CF97D-6BBB-44C2-8074-DC47F6C89E80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Sourcetree</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Has</t>
+  </si>
+  <si>
+    <t>VSCode</t>
   </si>
 </sst>
 </file>
@@ -103,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -111,12 +114,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,32 +425,44 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="3.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
+    <row r="1" spans="1:11" ht="55" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
       <c r="J2">
         <v>0</v>
       </c>
@@ -434,9 +471,14 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
       <c r="J3">
         <v>1</v>
       </c>
@@ -445,9 +487,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
       <c r="J4">
         <v>2</v>
       </c>
@@ -456,12 +503,16 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3">
         <v>4</v>
       </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
       <c r="J5">
         <v>3</v>
       </c>
@@ -470,9 +521,14 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
       <c r="J6">
         <v>4</v>
       </c>
@@ -481,8 +537,17 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3">
+        <v>4</v>
+      </c>
+      <c r="F7" s="3">
+        <v>4</v>
       </c>
       <c r="J7">
         <v>5</v>
@@ -492,12 +557,16 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
         <v>1</v>
       </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
Made arbitrary changes to spreadsheet.
</commit_message>
<xml_diff>
--- a/Git GUIs Eval.xlsx
+++ b/Git GUIs Eval.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5CF97D-6BBB-44C2-8074-DC47F6C89E80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F845960-99BC-491B-B5FD-06EDFCF540CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compare and Merge Eval" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Sourcetree</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>VSCode</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -425,18 +428,18 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="3.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="3.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="55" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="57" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -454,7 +457,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -470,15 +473,23 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="J3">
         <v>1</v>
       </c>
@@ -486,7 +497,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -502,7 +513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -520,7 +531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -536,7 +547,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -556,7 +567,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -568,12 +579,12 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>

</xml_diff>